<commit_message>
Added all the aero data
</commit_message>
<xml_diff>
--- a/inputs/aero_properties.xlsx
+++ b/inputs/aero_properties.xlsx
@@ -5,13 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="inboard" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="outboard" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="dihedral" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="tail" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Ctail" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="airfoil_indices" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="0Rtail" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="1Rtail" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="0Ltail" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="1Ltail" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="14">
   <si>
     <t xml:space="preserve">aero properties</t>
   </si>
@@ -55,7 +60,16 @@
     <t xml:space="preserve">na</t>
   </si>
   <si>
-    <t xml:space="preserve">flat</t>
+    <t xml:space="preserve">elastic_axis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% chord</t>
+  </si>
+  <si>
+    <t xml:space="preserve">naca0012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Airfoil</t>
   </si>
 </sst>
 </file>
@@ -70,6 +84,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -151,10 +166,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -204,6 +219,17 @@
       </c>
       <c r="C4" s="0" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.288</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -280,7 +306,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -351,7 +377,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -364,10 +390,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -402,7 +428,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -413,16 +439,406 @@
         <v>7</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Updated a lot of variables, missing some corrections from UM
</commit_message>
<xml_diff>
--- a/inputs/aero_properties.xlsx
+++ b/inputs/aero_properties.xlsx
@@ -5,21 +5,23 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="inboard" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="outboard" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="dihedral" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Ctail" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="0Rtail" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="1Rtail" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="0Ltail" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="1Ltail" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Cfin" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Lfin" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Rfin" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="airfoil_indices" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="RRfin" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="LLfin" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="inboard" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="outboard" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="dihedral" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Ctail" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="0Rtail" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="1Rtail" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="0Ltail" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="1Ltail" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Cfin" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Lfin" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Rfin" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="airfoil_indices" sheetId="14" state="visible" r:id="rId15"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="14">
   <si>
     <t xml:space="preserve">aero properties</t>
   </si>
@@ -57,19 +59,19 @@
     <t xml:space="preserve">airfoil</t>
   </si>
   <si>
+    <t xml:space="preserve">naca0012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">na</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elastic_axis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% chord</t>
+  </si>
+  <si>
     <t xml:space="preserve">emx07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">na</t>
-  </si>
-  <si>
-    <t xml:space="preserve">elastic_axis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% chord</t>
-  </si>
-  <si>
-    <t xml:space="preserve">naca0012</t>
   </si>
   <si>
     <t xml:space="preserve">Airfoil</t>
@@ -172,7 +174,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -196,7 +198,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>0.2</v>
+        <v>0.1219</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>4</v>
@@ -207,7 +209,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -229,7 +231,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0.288</v>
+        <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>11</v>
@@ -238,7 +240,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -254,7 +256,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -278,8 +280,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
-        <f aca="false">0.865</f>
-        <v>0.865</v>
+        <v>0.11</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>4</v>
@@ -301,7 +302,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>9</v>
@@ -312,7 +313,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0.27</v>
+        <v>0.25</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>11</v>
@@ -361,7 +362,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>0.865</v>
+        <v>1.1</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>4</v>
@@ -383,7 +384,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>9</v>
@@ -394,7 +395,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0.27</v>
+        <v>0.21</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>11</v>
@@ -416,61 +417,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -494,7 +444,8 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>0.2</v>
+        <f aca="false">0.865</f>
+        <v>0.865</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>4</v>
@@ -505,7 +456,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -522,6 +473,17 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -533,15 +495,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C4"/>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C95" activeCellId="0" sqref="C95"/>
+      <selection pane="topLeft" activeCell="I43" activeCellId="0" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -565,7 +527,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>0.2</v>
+        <v>0.865</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>4</v>
@@ -576,7 +538,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -593,6 +555,17 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -604,15 +577,66 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -636,7 +660,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>0.11</v>
+        <v>0.1219</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>4</v>
@@ -658,7 +682,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>9</v>
@@ -669,7 +693,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>11</v>
@@ -686,7 +710,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -694,7 +718,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F56" activeCellId="0" sqref="F56"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -718,7 +742,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>0.11</v>
+        <v>0.2</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>4</v>
@@ -751,7 +775,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0.25</v>
+        <v>0.288</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>11</v>
@@ -760,20 +784,20 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C5"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
@@ -800,7 +824,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>0.11</v>
+        <v>0.2</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>4</v>
@@ -828,6 +852,148 @@
         <v>9</v>
       </c>
     </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>10</v>
@@ -858,7 +1024,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="F56" activeCellId="0" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -904,7 +1070,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>9</v>
@@ -986,7 +1152,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>9</v>
@@ -1021,8 +1187,8 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1046,7 +1212,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>1.1</v>
+        <v>0.11</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>4</v>
@@ -1068,7 +1234,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>9</v>
@@ -1079,7 +1245,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0.21</v>
+        <v>0.25</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>11</v>

</xml_diff>